<commit_message>
v0.1.3 - avoid selecting multiple markers and countries
</commit_message>
<xml_diff>
--- a/project/todo_list.xlsx
+++ b/project/todo_list.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10911"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timvonasen/Documents/02_HfG/GitHub/2223ws-workshop-franklin/project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucaz\Documents\GitHub\2223ws-workshop-franklin\project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01A24C1A-A029-EE41-80CB-81BFEE5C1A73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1040" windowWidth="28800" windowHeight="12180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1035" windowWidth="28800" windowHeight="12180"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Todo</t>
   </si>
@@ -99,13 +98,19 @@
   </si>
   <si>
     <t>Data clearence (remove unused files)</t>
+  </si>
+  <si>
+    <t>Only one line for UdSSR and Russia</t>
+  </si>
+  <si>
+    <t>Bring back opacity of not selected lines</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -433,23 +438,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="40.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.83203125" style="1"/>
+    <col min="1" max="1" width="58.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" ht="15">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -463,7 +468,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -474,11 +479,11 @@
         <v>1</v>
       </c>
       <c r="D2" s="1">
-        <f t="shared" ref="D2:D13" si="0">AVERAGE(B2:C2)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+        <f>AVERAGE(B2:C2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -489,11 +494,11 @@
         <v>2</v>
       </c>
       <c r="D3" s="1">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+        <f t="shared" ref="D2:D13" si="0">AVERAGE(B3:C3)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -508,7 +513,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
@@ -523,7 +528,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -538,7 +543,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -553,7 +558,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -568,7 +573,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
@@ -583,7 +588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
@@ -598,7 +603,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
@@ -613,7 +618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:4">
       <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
@@ -628,7 +633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:4">
       <c r="A13" s="1" t="s">
         <v>20</v>
       </c>
@@ -643,7 +648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:4">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
@@ -658,7 +663,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:4">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
@@ -673,12 +678,32 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:4">
+      <c r="A16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="1">
+        <v>4</v>
+      </c>
+      <c r="C16" s="1">
+        <v>2</v>
+      </c>
+      <c r="D16" s="1">
+        <f>AVERAGE(B16:C16)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" customHeight="1">
       <c r="A21" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:4">
       <c r="A22" s="1" t="s">
         <v>2</v>
       </c>
@@ -693,7 +718,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:4">
       <c r="A23" s="1" t="s">
         <v>10</v>
       </c>
@@ -708,7 +733,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:4">
       <c r="A24" s="1" t="s">
         <v>3</v>
       </c>

</xml_diff>